<commit_message>
Order of questions in pigweb survey
</commit_message>
<xml_diff>
--- a/OrderOfQuestions.xlsx
+++ b/OrderOfQuestions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>Information about your research and role in research. : When was the last occasion that you published or submitted a manuscript to a journal?</t>
   </si>
@@ -176,48 +176,9 @@
     <t>Questions about your usage of other data sources (part 2) : Where have you previously obtained research data which has been collected by other research groups, for your own reuse?(Please select all that apply) : Directly from the researcher who collected the data (e.g. via email)</t>
   </si>
   <si>
-    <t>Questions about your usage of other data sources (part 2) : Where have you previously obtained research data which has been collected by other research groups, for your own reuse?(Please select all that apply) : Downloaded directly from a data repository</t>
-  </si>
-  <si>
-    <t>Questions about your usage of other data sources (part 2) : Where have you previously obtained research data which has been collected by other research groups, for your own reuse?(Please select all that apply) : Data were available within a published research article</t>
-  </si>
-  <si>
-    <t>Questions about your usage of other data sources (part 2) : Where have you previously obtained research data which has been collected by other research groups, for your own reuse?(Please select all that apply) : Data were linked from a published data article</t>
-  </si>
-  <si>
-    <t>Questions about your usage of other data sources (part 2) : Where have you previously obtained research data which has been collected by other research groups, for your own reuse?(Please select all that apply) : Data were available from a blog post</t>
-  </si>
-  <si>
-    <t>Questions about your usage of other data sources (part 2) : Where have you previously obtained research data which has been collected by other research groups, for your own reuse?(Please select all that apply) : I don't know</t>
-  </si>
-  <si>
-    <t>Questions about your usage of other data sources (part 2) : Where have you previously obtained research data which has been collected by other research groups, for your own reuse?(Please select all that apply) : Other (please specify)</t>
-  </si>
-  <si>
-    <t>Questions about your usage of other data sources (part 2) : Other (please specify)...147</t>
-  </si>
-  <si>
     <t>Questions about your usage of other data sources (part 2) : What was your aim in using previously generated data?(Please select all that apply) : Replication studies (use of the data as a reference to determine whether they can be repeated under similar conditions)</t>
   </si>
   <si>
-    <t>Questions about your usage of other data sources (part 2) : What was your aim in using previously generated data?(Please select all that apply) : Reanalysis (analysing the data set using a different method to test the same research question)</t>
-  </si>
-  <si>
-    <t>Questions about your usage of other data sources (part 2) : What was your aim in using previously generated data?(Please select all that apply) : Reinterpretation (using the data as is to answer another question)</t>
-  </si>
-  <si>
-    <t>Questions about your usage of other data sources (part 2) : What was your aim in using previously generated data?(Please select all that apply) : Isolated reuse (reanalysing the data to answer a new question)</t>
-  </si>
-  <si>
-    <t>Questions about your usage of other data sources (part 2) : What was your aim in using previously generated data?(Please select all that apply) : Combination reuse (reanalysing the data in combination with other data sets to answer a new question)</t>
-  </si>
-  <si>
-    <t>Questions about your usage of other data sources (part 2) : What was your aim in using previously generated data?(Please select all that apply) : Other (please specify)</t>
-  </si>
-  <si>
-    <t>Questions about your usage of other data sources (part 2) : Other (please specify)...154</t>
-  </si>
-  <si>
     <t>Questions about your usage of other data sources (part 2) : We would now like to ask you to think about the last occasion on which you tried to get access to a data set produced by another research group. Please answer the following questions with this experience in mind.How did you gain access to the data set?</t>
   </si>
   <si>
@@ -227,27 +188,6 @@
     <t>Questions about your usage of other data sources (part 2) : What was included in the data set? : Data file outputs</t>
   </si>
   <si>
-    <t>Questions about your usage of other data sources (part 2) : What was included in the data set? : Metadata about the data</t>
-  </si>
-  <si>
-    <t>Questions about your usage of other data sources (part 2) : What was included in the data set? : A README file</t>
-  </si>
-  <si>
-    <t>Questions about your usage of other data sources (part 2) : What was included in the data set? : Code</t>
-  </si>
-  <si>
-    <t>Questions about your usage of other data sources (part 2) : What was included in the data set? : Software requirements</t>
-  </si>
-  <si>
-    <t>Questions about your usage of other data sources (part 2) : What was included in the data set? : License under which the data could be used</t>
-  </si>
-  <si>
-    <t>Questions about your usage of other data sources (part 2) : What was included in the data set? : Additional annotations of the data file</t>
-  </si>
-  <si>
-    <t>Questions about your usage of other data sources (part 2) : What was included in the data set? : None of the above</t>
-  </si>
-  <si>
     <t>Questions about your usage of other data sources (part 2) : Were you able to get access to the data set?</t>
   </si>
   <si>
@@ -266,94 +206,13 @@
     <t>Credit and recognition for data sharing : What circumstances would motivate you to share your data?(Please select all that apply) : Full data citation</t>
   </si>
   <si>
-    <t>Credit and recognition for data sharing : What circumstances would motivate you to share your data?(Please select all that apply) : Citation of my research papers</t>
-  </si>
-  <si>
-    <t>Credit and recognition for data sharing : What circumstances would motivate you to share your data?(Please select all that apply) : Co-authorship on papers</t>
-  </si>
-  <si>
-    <t>Credit and recognition for data sharing : What circumstances would motivate you to share your data?(Please select all that apply) : Financial reward</t>
-  </si>
-  <si>
-    <t>Credit and recognition for data sharing : What circumstances would motivate you to share your data?(Please select all that apply) : Open data badge</t>
-  </si>
-  <si>
-    <t>Credit and recognition for data sharing : What circumstances would motivate you to share your data?(Please select all that apply) : Consideration in job reviews and funding applications</t>
-  </si>
-  <si>
-    <t>Credit and recognition for data sharing : What circumstances would motivate you to share your data?(Please select all that apply) : Funder requirement</t>
-  </si>
-  <si>
-    <t>Credit and recognition for data sharing : What circumstances would motivate you to share your data?(Please select all that apply) : Journal/Publisher requirement</t>
-  </si>
-  <si>
-    <t>Credit and recognition for data sharing : What circumstances would motivate you to share your data?(Please select all that apply) : Institution/Organisation requirement</t>
-  </si>
-  <si>
-    <t>Credit and recognition for data sharing : What circumstances would motivate you to share your data?(Please select all that apply) : Public benefit</t>
-  </si>
-  <si>
-    <t>Credit and recognition for data sharing : What circumstances would motivate you to share your data?(Please select all that apply) : Increased impact and visibility of my research</t>
-  </si>
-  <si>
-    <t>Credit and recognition for data sharing : What circumstances would motivate you to share your data?(Please select all that apply) : Greater transparency and reuse</t>
-  </si>
-  <si>
-    <t>Credit and recognition for data sharing : What circumstances would motivate you to share your data?(Please select all that apply) : Freedom of information request</t>
-  </si>
-  <si>
-    <t>Credit and recognition for data sharing : What circumstances would motivate you to share your data?(Please select all that apply) : Direct request from another research</t>
-  </si>
-  <si>
-    <t>Credit and recognition for data sharing : What circumstances would motivate you to share your data?(Please select all that apply) : It was made simple and easy to do</t>
-  </si>
-  <si>
-    <t>Credit and recognition for data sharing : What circumstances would motivate you to share your data?(Please select all that apply) : It was a field/industry expectation</t>
-  </si>
-  <si>
-    <t>Credit and recognition for data sharing : What circumstances would motivate you to share your data?(Please select all that apply) : I would never share my data</t>
-  </si>
-  <si>
-    <t>Credit and recognition for data sharing : What circumstances would motivate you to share your data?(Please select all that apply) : Other (please specify)</t>
-  </si>
-  <si>
     <t>Credit and recognition for data sharing : Which one of the circumstances would motivate you the most to share your data?(The list below is the same as on the previous question, select the one which would motivate you the most).</t>
   </si>
   <si>
-    <t>Credit and recognition for data sharing : Other (please specify)...189</t>
-  </si>
-  <si>
     <t>Credit and recognition for data sharing : If the reuse of your data in a subsequent paper resulted in you being credited as a co-author, how much would this motivate you to make your data openly available to others?</t>
   </si>
   <si>
     <t>Credit and recognition for data sharing : What recognition have you received for sharing your research data?(Please select all that apply) : Full citation in another article</t>
-  </si>
-  <si>
-    <t>Credit and recognition for data sharing : What recognition have you received for sharing your research data?(Please select all that apply) : Co-authorship on a paper which used my data</t>
-  </si>
-  <si>
-    <t>Credit and recognition for data sharing : What recognition have you received for sharing your research data?(Please select all that apply) : Financial reward</t>
-  </si>
-  <si>
-    <t>Credit and recognition for data sharing : What recognition have you received for sharing your research data?(Please select all that apply) : Consideration of data sharing in a job review</t>
-  </si>
-  <si>
-    <t>Credit and recognition for data sharing : What recognition have you received for sharing your research data?(Please select all that apply) : Consideration of data sharing in a grant application</t>
-  </si>
-  <si>
-    <t>Credit and recognition for data sharing : What recognition have you received for sharing your research data?(Please select all that apply) : Open data badge</t>
-  </si>
-  <si>
-    <t>Credit and recognition for data sharing : What recognition have you received for sharing your research data?(Please select all that apply) : I don't know</t>
-  </si>
-  <si>
-    <t>Credit and recognition for data sharing : What recognition have you received for sharing your research data?(Please select all that apply) : I've never received credit</t>
-  </si>
-  <si>
-    <t>Credit and recognition for data sharing : What recognition have you received for sharing your research data?(Please select all that apply) : Other (please specify)</t>
-  </si>
-  <si>
-    <t>Credit and recognition for data sharing : Other (please specify)...200</t>
   </si>
   <si>
     <t>Credit and recognition for data sharing : How supportive would you be of a national mandate for making research data openly available?[Note: by open we mean free to access, reuse, repurpose and redistribute)</t>
@@ -705,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A116"/>
+  <dimension ref="A1:A69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60:XFD69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,419 +740,184 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+    <row r="41" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+    <row r="42" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+    <row r="43" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+    <row r="45" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+    <row r="46" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+    <row r="47" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+    <row r="48" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+    <row r="49" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+    <row r="53" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+    <row r="54" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+    <row r="55" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+    <row r="56" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+    <row r="57" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+    <row r="58" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+    <row r="59" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+    <row r="60" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+    <row r="61" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+    <row r="62" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+    <row r="63" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+    <row r="64" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+    <row r="65" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+    <row r="66" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+    <row r="67" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+    <row r="68" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+    <row r="69" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>